<commit_message>
added Carson and Collin primaries
</commit_message>
<xml_diff>
--- a/2020/primary/HOWARD_COUNTY-2020_MARCH_3RD_REPUBLICAN_PRIMARY_332020-Rep pct x pct_HowardCounty.xlsx
+++ b/2020/primary/HOWARD_COUNTY-2020_MARCH_3RD_REPUBLICAN_PRIMARY_332020-Rep pct x pct_HowardCounty.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jodi Duck\Documents\2020 ELECTIONS\Primary 2020\Canvass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekwillis/code/openelections-sources-tx/2020/primary/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7FBB84-53F5-0642-8F85-9A3A9B2BF78C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="2700" yWindow="3300" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -326,7 +327,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,16 +638,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M355"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -662,29 +678,29 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -722,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -760,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -798,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -836,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -874,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -912,7 +928,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -950,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -988,7 +1004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>26</v>
       </c>
@@ -1026,7 +1042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>27</v>
       </c>
@@ -1064,7 +1080,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>28</v>
       </c>
@@ -1102,7 +1118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>29</v>
       </c>
@@ -1140,7 +1156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>30</v>
       </c>
@@ -1178,7 +1194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>43</v>
       </c>
@@ -1216,7 +1232,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>44</v>
       </c>
@@ -1254,7 +1270,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>46</v>
       </c>
@@ -1292,7 +1308,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>47</v>
       </c>
@@ -1330,7 +1346,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>54</v>
       </c>
@@ -1368,7 +1384,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>55</v>
       </c>
@@ -1406,7 +1422,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>58</v>
       </c>
@@ -1444,7 +1460,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>61</v>
       </c>
@@ -1482,7 +1498,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>64</v>
       </c>
@@ -1520,7 +1536,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>65</v>
       </c>
@@ -1558,7 +1574,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>69</v>
       </c>
@@ -1596,7 +1612,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>72</v>
       </c>
@@ -1634,7 +1650,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>74</v>
       </c>
@@ -1672,7 +1688,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>76</v>
       </c>
@@ -1710,7 +1726,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>77</v>
       </c>
@@ -1748,7 +1764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>78</v>
       </c>
@@ -1786,7 +1802,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>79</v>
       </c>
@@ -1824,7 +1840,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>80</v>
       </c>
@@ -1862,7 +1878,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>81</v>
       </c>
@@ -1900,7 +1916,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>82</v>
       </c>
@@ -1938,7 +1954,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>83</v>
       </c>
@@ -1976,7 +1992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>84</v>
       </c>
@@ -2014,7 +2030,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>85</v>
       </c>
@@ -2052,7 +2068,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>86</v>
       </c>
@@ -2090,7 +2106,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>87</v>
       </c>
@@ -2128,7 +2144,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>89</v>
       </c>
@@ -2166,7 +2182,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>91</v>
       </c>
@@ -2204,7 +2220,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>92</v>
       </c>
@@ -2242,7 +2258,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>93</v>
       </c>
@@ -2280,7 +2296,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>95</v>
       </c>
@@ -2318,7 +2334,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>96</v>
       </c>
@@ -2356,7 +2372,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>97</v>
       </c>
@@ -2394,7 +2410,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>98</v>
       </c>
@@ -2432,7 +2448,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>99</v>
       </c>
@@ -2470,7 +2486,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>100</v>
       </c>
@@ -2508,7 +2524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>101</v>
       </c>
@@ -2546,7 +2562,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>102</v>
       </c>
@@ -2584,7 +2600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>103</v>
       </c>
@@ -2622,7 +2638,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>104</v>
       </c>
@@ -2660,7 +2676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>105</v>
       </c>
@@ -2698,7 +2714,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>106</v>
       </c>
@@ -2736,7 +2752,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>107</v>
       </c>
@@ -2774,7 +2790,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>108</v>
       </c>
@@ -2812,7 +2828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>109</v>
       </c>
@@ -2850,7 +2866,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>110</v>
       </c>
@@ -2888,7 +2904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>111</v>
       </c>
@@ -2926,7 +2942,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>112</v>
       </c>
@@ -2964,7 +2980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>113</v>
       </c>
@@ -3002,7 +3018,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>114</v>
       </c>
@@ -3040,7 +3056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>137</v>
       </c>
@@ -3078,7 +3094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>138</v>
       </c>
@@ -3116,7 +3132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>139</v>
       </c>
@@ -3154,7 +3170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>140</v>
       </c>
@@ -3192,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>141</v>
       </c>
@@ -3230,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>142</v>
       </c>
@@ -3268,7 +3284,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>143</v>
       </c>
@@ -3306,7 +3322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>144</v>
       </c>
@@ -3344,7 +3360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>162</v>
       </c>
@@ -3382,7 +3398,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>163</v>
       </c>
@@ -3420,7 +3436,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>164</v>
       </c>
@@ -3458,7 +3474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>165</v>
       </c>
@@ -3496,7 +3512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>166</v>
       </c>
@@ -3534,7 +3550,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>179</v>
       </c>
@@ -3572,7 +3588,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>180</v>
       </c>
@@ -3610,7 +3626,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>182</v>
       </c>
@@ -3648,7 +3664,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>183</v>
       </c>
@@ -3686,7 +3702,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>190</v>
       </c>
@@ -3724,7 +3740,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>191</v>
       </c>
@@ -3762,7 +3778,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>194</v>
       </c>
@@ -3800,7 +3816,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>197</v>
       </c>
@@ -3838,7 +3854,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>200</v>
       </c>
@@ -3876,7 +3892,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>201</v>
       </c>
@@ -3914,7 +3930,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>205</v>
       </c>
@@ -3952,7 +3968,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>208</v>
       </c>
@@ -3990,7 +4006,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>210</v>
       </c>
@@ -4028,7 +4044,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>212</v>
       </c>
@@ -4066,7 +4082,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>213</v>
       </c>
@@ -4104,7 +4120,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>214</v>
       </c>
@@ -4142,7 +4158,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>215</v>
       </c>
@@ -4180,7 +4196,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>216</v>
       </c>
@@ -4218,7 +4234,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>217</v>
       </c>
@@ -4256,7 +4272,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>218</v>
       </c>
@@ -4294,7 +4310,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>219</v>
       </c>
@@ -4332,7 +4348,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>220</v>
       </c>
@@ -4370,7 +4386,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>221</v>
       </c>
@@ -4408,7 +4424,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>222</v>
       </c>
@@ -4446,7 +4462,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>223</v>
       </c>
@@ -4484,7 +4500,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>224</v>
       </c>
@@ -4522,7 +4538,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>226</v>
       </c>
@@ -4560,7 +4576,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>227</v>
       </c>
@@ -4598,7 +4614,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>228</v>
       </c>
@@ -4636,7 +4652,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>229</v>
       </c>
@@ -4674,7 +4690,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>230</v>
       </c>
@@ -4712,7 +4728,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>231</v>
       </c>
@@ -4750,7 +4766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>232</v>
       </c>
@@ -4788,7 +4804,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>233</v>
       </c>
@@ -4826,7 +4842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>234</v>
       </c>
@@ -4864,7 +4880,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>235</v>
       </c>
@@ -4902,7 +4918,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>236</v>
       </c>
@@ -4940,7 +4956,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>237</v>
       </c>
@@ -4978,7 +4994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>238</v>
       </c>
@@ -5016,7 +5032,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>239</v>
       </c>
@@ -5054,7 +5070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>240</v>
       </c>
@@ -5092,7 +5108,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>241</v>
       </c>
@@ -5130,7 +5146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>242</v>
       </c>
@@ -5168,7 +5184,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>243</v>
       </c>
@@ -5206,7 +5222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>244</v>
       </c>
@@ -5244,7 +5260,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>245</v>
       </c>
@@ -5282,7 +5298,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>268</v>
       </c>
@@ -5320,7 +5336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>269</v>
       </c>
@@ -5358,7 +5374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>270</v>
       </c>
@@ -5396,7 +5412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>271</v>
       </c>
@@ -5434,7 +5450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>272</v>
       </c>
@@ -5472,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>273</v>
       </c>
@@ -5510,7 +5526,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>274</v>
       </c>
@@ -5548,7 +5564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>275</v>
       </c>
@@ -5586,7 +5602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>293</v>
       </c>
@@ -5624,7 +5640,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>294</v>
       </c>
@@ -5662,7 +5678,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>295</v>
       </c>
@@ -5700,7 +5716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>296</v>
       </c>
@@ -5738,7 +5754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>297</v>
       </c>
@@ -5776,7 +5792,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>310</v>
       </c>
@@ -5814,7 +5830,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>311</v>
       </c>
@@ -5852,7 +5868,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>313</v>
       </c>
@@ -5890,7 +5906,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>314</v>
       </c>
@@ -5928,7 +5944,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>321</v>
       </c>
@@ -5966,7 +5982,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>322</v>
       </c>
@@ -6004,7 +6020,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>325</v>
       </c>
@@ -6042,7 +6058,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>328</v>
       </c>
@@ -6080,7 +6096,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>331</v>
       </c>
@@ -6118,7 +6134,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>332</v>
       </c>
@@ -6156,7 +6172,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>336</v>
       </c>
@@ -6194,7 +6210,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>339</v>
       </c>
@@ -6232,7 +6248,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>341</v>
       </c>
@@ -6270,7 +6286,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>343</v>
       </c>
@@ -6308,7 +6324,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>344</v>
       </c>
@@ -6346,7 +6362,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>345</v>
       </c>
@@ -6384,7 +6400,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>346</v>
       </c>
@@ -6422,7 +6438,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>347</v>
       </c>
@@ -6460,7 +6476,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>348</v>
       </c>
@@ -6498,7 +6514,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>349</v>
       </c>
@@ -6536,7 +6552,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>350</v>
       </c>
@@ -6574,7 +6590,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>351</v>
       </c>
@@ -6612,7 +6628,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>352</v>
       </c>
@@ -6650,7 +6666,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>353</v>
       </c>
@@ -6688,7 +6704,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>355</v>
       </c>
@@ -6726,7 +6742,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>356</v>
       </c>
@@ -6764,7 +6780,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>357</v>
       </c>
@@ -6802,7 +6818,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>358</v>
       </c>
@@ -6840,7 +6856,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>359</v>
       </c>
@@ -6878,7 +6894,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>360</v>
       </c>
@@ -6916,7 +6932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>361</v>
       </c>
@@ -6954,7 +6970,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>362</v>
       </c>
@@ -6992,7 +7008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>363</v>
       </c>
@@ -7030,7 +7046,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>364</v>
       </c>
@@ -7068,7 +7084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>365</v>
       </c>
@@ -7106,7 +7122,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>366</v>
       </c>
@@ -7144,7 +7160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>367</v>
       </c>
@@ -7182,7 +7198,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>368</v>
       </c>
@@ -7220,7 +7236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>369</v>
       </c>
@@ -7258,7 +7274,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>370</v>
       </c>
@@ -7296,7 +7312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>371</v>
       </c>
@@ -7334,7 +7350,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>372</v>
       </c>
@@ -7372,7 +7388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>373</v>
       </c>
@@ -7410,7 +7426,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>374</v>
       </c>
@@ -7448,7 +7464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>397</v>
       </c>
@@ -7486,7 +7502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>398</v>
       </c>
@@ -7524,7 +7540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>399</v>
       </c>
@@ -7562,7 +7578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>400</v>
       </c>
@@ -7600,7 +7616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>401</v>
       </c>
@@ -7638,7 +7654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>402</v>
       </c>
@@ -7676,7 +7692,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>403</v>
       </c>
@@ -7714,7 +7730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>404</v>
       </c>
@@ -7752,7 +7768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>422</v>
       </c>
@@ -7790,7 +7806,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>423</v>
       </c>
@@ -7828,7 +7844,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>424</v>
       </c>
@@ -7866,7 +7882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>425</v>
       </c>
@@ -7904,7 +7920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>426</v>
       </c>
@@ -7942,7 +7958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>439</v>
       </c>
@@ -7980,7 +7996,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>440</v>
       </c>
@@ -8018,7 +8034,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>442</v>
       </c>
@@ -8056,7 +8072,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>443</v>
       </c>
@@ -8094,7 +8110,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>450</v>
       </c>
@@ -8132,7 +8148,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>451</v>
       </c>
@@ -8170,7 +8186,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>454</v>
       </c>
@@ -8208,7 +8224,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>457</v>
       </c>
@@ -8246,7 +8262,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>460</v>
       </c>
@@ -8284,7 +8300,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>461</v>
       </c>
@@ -8322,7 +8338,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>465</v>
       </c>
@@ -8360,7 +8376,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>468</v>
       </c>
@@ -8398,7 +8414,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>470</v>
       </c>
@@ -8436,7 +8452,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>472</v>
       </c>
@@ -8474,7 +8490,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>473</v>
       </c>
@@ -8512,7 +8528,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>474</v>
       </c>
@@ -8550,7 +8566,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>475</v>
       </c>
@@ -8588,7 +8604,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>476</v>
       </c>
@@ -8626,7 +8642,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>477</v>
       </c>
@@ -8664,7 +8680,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>478</v>
       </c>
@@ -8702,7 +8718,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>479</v>
       </c>
@@ -8740,7 +8756,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>480</v>
       </c>
@@ -8778,7 +8794,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>481</v>
       </c>
@@ -8816,7 +8832,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>482</v>
       </c>
@@ -8854,7 +8870,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>484</v>
       </c>
@@ -8892,7 +8908,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>485</v>
       </c>
@@ -8930,7 +8946,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>486</v>
       </c>
@@ -8968,7 +8984,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>488</v>
       </c>
@@ -9006,7 +9022,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>489</v>
       </c>
@@ -9044,7 +9060,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>490</v>
       </c>
@@ -9082,7 +9098,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>491</v>
       </c>
@@ -9120,7 +9136,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>492</v>
       </c>
@@ -9158,7 +9174,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>493</v>
       </c>
@@ -9196,7 +9212,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>494</v>
       </c>
@@ -9234,7 +9250,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>495</v>
       </c>
@@ -9272,7 +9288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>496</v>
       </c>
@@ -9310,7 +9326,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>497</v>
       </c>
@@ -9348,7 +9364,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>498</v>
       </c>
@@ -9386,7 +9402,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>499</v>
       </c>
@@ -9424,7 +9440,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>500</v>
       </c>
@@ -9462,7 +9478,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>501</v>
       </c>
@@ -9500,7 +9516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>502</v>
       </c>
@@ -9538,7 +9554,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>503</v>
       </c>
@@ -9576,7 +9592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>504</v>
       </c>
@@ -9614,7 +9630,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>505</v>
       </c>
@@ -9652,7 +9668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>506</v>
       </c>
@@ -9690,7 +9706,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>507</v>
       </c>
@@ -9728,7 +9744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>530</v>
       </c>
@@ -9766,7 +9782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>531</v>
       </c>
@@ -9804,7 +9820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>532</v>
       </c>
@@ -9842,7 +9858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>533</v>
       </c>
@@ -9880,7 +9896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>534</v>
       </c>
@@ -9918,7 +9934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>535</v>
       </c>
@@ -9956,7 +9972,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>536</v>
       </c>
@@ -9994,7 +10010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>537</v>
       </c>
@@ -10032,7 +10048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>555</v>
       </c>
@@ -10070,7 +10086,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>556</v>
       </c>
@@ -10108,7 +10124,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>557</v>
       </c>
@@ -10146,7 +10162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>558</v>
       </c>
@@ -10184,7 +10200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>559</v>
       </c>
@@ -10222,7 +10238,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>572</v>
       </c>
@@ -10260,7 +10276,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>573</v>
       </c>
@@ -10298,7 +10314,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>575</v>
       </c>
@@ -10336,7 +10352,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>576</v>
       </c>
@@ -10374,7 +10390,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>583</v>
       </c>
@@ -10412,7 +10428,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>584</v>
       </c>
@@ -10450,7 +10466,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>587</v>
       </c>
@@ -10488,7 +10504,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>590</v>
       </c>
@@ -10526,7 +10542,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>593</v>
       </c>
@@ -10564,7 +10580,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>594</v>
       </c>
@@ -10602,7 +10618,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>598</v>
       </c>
@@ -10640,7 +10656,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>601</v>
       </c>
@@ -10678,7 +10694,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>603</v>
       </c>
@@ -10716,7 +10732,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>605</v>
       </c>
@@ -10754,7 +10770,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>606</v>
       </c>
@@ -10792,7 +10808,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>607</v>
       </c>
@@ -10830,7 +10846,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>608</v>
       </c>
@@ -10868,7 +10884,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>609</v>
       </c>
@@ -10906,7 +10922,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>610</v>
       </c>
@@ -10944,7 +10960,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>611</v>
       </c>
@@ -10982,7 +10998,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>612</v>
       </c>
@@ -11020,7 +11036,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>613</v>
       </c>
@@ -11058,7 +11074,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>614</v>
       </c>
@@ -11096,7 +11112,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>615</v>
       </c>
@@ -11134,7 +11150,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>616</v>
       </c>
@@ -11172,7 +11188,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>617</v>
       </c>
@@ -11210,7 +11226,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>619</v>
       </c>
@@ -11248,7 +11264,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>620</v>
       </c>
@@ -11286,7 +11302,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>621</v>
       </c>
@@ -11324,7 +11340,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>622</v>
       </c>
@@ -11362,7 +11378,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>623</v>
       </c>
@@ -11400,7 +11416,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>624</v>
       </c>
@@ -11438,7 +11454,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>625</v>
       </c>
@@ -11476,7 +11492,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>626</v>
       </c>
@@ -11514,7 +11530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>627</v>
       </c>
@@ -11552,7 +11568,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>628</v>
       </c>
@@ -11590,7 +11606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>629</v>
       </c>
@@ -11628,7 +11644,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>630</v>
       </c>
@@ -11666,7 +11682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>631</v>
       </c>
@@ -11704,7 +11720,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>632</v>
       </c>
@@ -11742,7 +11758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>633</v>
       </c>
@@ -11780,7 +11796,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>634</v>
       </c>
@@ -11818,7 +11834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>635</v>
       </c>
@@ -11856,7 +11872,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>636</v>
       </c>
@@ -11894,7 +11910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>637</v>
       </c>
@@ -11932,7 +11948,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>638</v>
       </c>
@@ -11970,7 +11986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>661</v>
       </c>
@@ -12008,7 +12024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>662</v>
       </c>
@@ -12046,7 +12062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>663</v>
       </c>
@@ -12084,7 +12100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>664</v>
       </c>
@@ -12122,7 +12138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>665</v>
       </c>
@@ -12160,7 +12176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>666</v>
       </c>
@@ -12198,7 +12214,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>667</v>
       </c>
@@ -12236,7 +12252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>668</v>
       </c>
@@ -12274,7 +12290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>686</v>
       </c>
@@ -12312,7 +12328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>687</v>
       </c>
@@ -12350,7 +12366,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>688</v>
       </c>
@@ -12388,7 +12404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>689</v>
       </c>
@@ -12426,7 +12442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>690</v>
       </c>
@@ -12464,7 +12480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>703</v>
       </c>
@@ -12502,7 +12518,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>704</v>
       </c>
@@ -12540,7 +12556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>706</v>
       </c>
@@ -12578,7 +12594,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>707</v>
       </c>
@@ -12616,7 +12632,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>714</v>
       </c>
@@ -12654,7 +12670,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>715</v>
       </c>
@@ -12692,7 +12708,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>718</v>
       </c>
@@ -12730,7 +12746,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>721</v>
       </c>
@@ -12768,7 +12784,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>724</v>
       </c>
@@ -12806,7 +12822,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>725</v>
       </c>
@@ -12844,7 +12860,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>729</v>
       </c>
@@ -12882,7 +12898,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>732</v>
       </c>
@@ -12920,7 +12936,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>734</v>
       </c>
@@ -12958,7 +12974,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>736</v>
       </c>
@@ -12996,7 +13012,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>737</v>
       </c>
@@ -13034,7 +13050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>738</v>
       </c>
@@ -13072,7 +13088,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>739</v>
       </c>
@@ -13110,7 +13126,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>740</v>
       </c>
@@ -13148,7 +13164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>741</v>
       </c>
@@ -13186,7 +13202,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>742</v>
       </c>
@@ -13224,7 +13240,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>743</v>
       </c>
@@ -13262,7 +13278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>744</v>
       </c>
@@ -13300,7 +13316,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>745</v>
       </c>
@@ -13338,7 +13354,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>746</v>
       </c>
@@ -13376,7 +13392,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>748</v>
       </c>
@@ -13414,7 +13430,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>749</v>
       </c>
@@ -13452,7 +13468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>750</v>
       </c>
@@ -13490,7 +13506,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>751</v>
       </c>
@@ -13528,7 +13544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>752</v>
       </c>
@@ -13566,7 +13582,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>753</v>
       </c>
@@ -13604,7 +13620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>754</v>
       </c>
@@ -13642,7 +13658,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>755</v>
       </c>
@@ -13680,7 +13696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>756</v>
       </c>
@@ -13718,7 +13734,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>757</v>
       </c>
@@ -13756,7 +13772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>758</v>
       </c>
@@ -13794,7 +13810,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>759</v>
       </c>
@@ -13832,7 +13848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>760</v>
       </c>
@@ -13870,7 +13886,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>761</v>
       </c>
@@ -13908,7 +13924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>762</v>
       </c>
@@ -13946,7 +13962,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>763</v>
       </c>
@@ -13984,7 +14000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>764</v>
       </c>
@@ -14022,7 +14038,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>765</v>
       </c>
@@ -14060,7 +14076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>766</v>
       </c>
@@ -14098,7 +14114,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>767</v>
       </c>

</xml_diff>